<commit_message>
processamnto de vários lis e interface (basica)
</commit_message>
<xml_diff>
--- a/Simulation_Result/Resultados_Simulacao_1.xlsx
+++ b/Simulation_Result/Resultados_Simulacao_1.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,13 +483,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B2" t="n">
-        <v>1.15</v>
+        <v>1.55</v>
       </c>
       <c r="C2" t="n">
-        <v>492959.811</v>
+        <v>664424.093</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -503,381 +503,181 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="C3" t="n">
-        <v>514392.846</v>
+        <v>685857.128</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="F3" t="n">
-        <v>99.666667</v>
+        <v>9.666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
-        <v>1.25</v>
+        <v>1.65</v>
       </c>
       <c r="C4" t="n">
-        <v>535825.8810000001</v>
+        <v>707290.1629999999</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>290</v>
       </c>
       <c r="F4" t="n">
-        <v>99.333333</v>
+        <v>3.333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" t="n">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="C5" t="n">
-        <v>557258.917</v>
+        <v>728723.199</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>292</v>
       </c>
       <c r="F5" t="n">
-        <v>98.333333</v>
+        <v>2.666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B6" t="n">
-        <v>1.35</v>
+        <v>1.75</v>
       </c>
       <c r="C6" t="n">
-        <v>578691.952</v>
+        <v>750156.2340000001</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="F6" t="n">
-        <v>96.333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B7" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="C7" t="n">
-        <v>600124.987</v>
+        <v>771589.269</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>15</v>
+        <v>294</v>
       </c>
       <c r="F7" t="n">
-        <v>95</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B8" t="n">
-        <v>1.45</v>
+        <v>1.85</v>
       </c>
       <c r="C8" t="n">
-        <v>621558.022</v>
+        <v>793022.304</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>295</v>
       </c>
       <c r="F8" t="n">
-        <v>93.333333</v>
+        <v>1.666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" t="n">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="C9" t="n">
-        <v>642991.058</v>
+        <v>814455.34</v>
       </c>
       <c r="D9" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>31</v>
+        <v>299</v>
       </c>
       <c r="F9" t="n">
-        <v>89.666667</v>
+        <v>0.333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" t="n">
-        <v>1.55</v>
+        <v>1.95</v>
       </c>
       <c r="C10" t="n">
-        <v>664424.093</v>
+        <v>835888.375</v>
       </c>
       <c r="D10" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>52</v>
+        <v>299</v>
       </c>
       <c r="F10" t="n">
-        <v>82.666667</v>
+        <v>0.333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B11" t="n">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>685857.128</v>
+        <v>857321.41</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>72</v>
+        <v>300</v>
       </c>
       <c r="F11" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>33</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="C12" t="n">
-        <v>707290.1629999999</v>
-      </c>
-      <c r="D12" t="n">
-        <v>40</v>
-      </c>
-      <c r="E12" t="n">
-        <v>112</v>
-      </c>
-      <c r="F12" t="n">
-        <v>62.666667</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>34</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="C13" t="n">
-        <v>728723.199</v>
-      </c>
-      <c r="D13" t="n">
-        <v>43</v>
-      </c>
-      <c r="E13" t="n">
-        <v>155</v>
-      </c>
-      <c r="F13" t="n">
-        <v>48.333333</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>35</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="C14" t="n">
-        <v>750156.2340000001</v>
-      </c>
-      <c r="D14" t="n">
-        <v>39</v>
-      </c>
-      <c r="E14" t="n">
-        <v>194</v>
-      </c>
-      <c r="F14" t="n">
-        <v>35.333333</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>36</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="C15" t="n">
-        <v>771589.269</v>
-      </c>
-      <c r="D15" t="n">
-        <v>47</v>
-      </c>
-      <c r="E15" t="n">
-        <v>241</v>
-      </c>
-      <c r="F15" t="n">
-        <v>19.666667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>37</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1.85</v>
-      </c>
-      <c r="C16" t="n">
-        <v>793022.304</v>
-      </c>
-      <c r="D16" t="n">
-        <v>20</v>
-      </c>
-      <c r="E16" t="n">
-        <v>261</v>
-      </c>
-      <c r="F16" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>38</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="C17" t="n">
-        <v>814455.34</v>
-      </c>
-      <c r="D17" t="n">
-        <v>26</v>
-      </c>
-      <c r="E17" t="n">
-        <v>287</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4.333333</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>39</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="C18" t="n">
-        <v>835888.375</v>
-      </c>
-      <c r="D18" t="n">
-        <v>6</v>
-      </c>
-      <c r="E18" t="n">
-        <v>293</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2.333333</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>40</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" t="n">
-        <v>857321.41</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="n">
-        <v>294</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>41</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="C20" t="n">
-        <v>878754.4449999999</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" t="n">
-        <v>296</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1.333333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>42</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>900187.481</v>
-      </c>
-      <c r="D21" t="n">
-        <v>4</v>
-      </c>
-      <c r="E21" t="n">
-        <v>300</v>
-      </c>
-      <c r="F21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -924,10 +724,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1.68466667</v>
+        <v>1.586</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.68640614</v>
+        <v>1.59964919</v>
       </c>
     </row>
     <row r="3">
@@ -937,10 +737,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.023183835</v>
+        <v>0.00220301003</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0230982802</v>
+        <v>0.00193312182</v>
       </c>
     </row>
     <row r="4">
@@ -950,10 +750,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.152262389</v>
+        <v>0.0469362337</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.151981184</v>
+        <v>0.0439672813</v>
       </c>
     </row>
     <row r="6">
@@ -1015,34 +815,34 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>1.709666666666667</v>
+        <v>1.611</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.02310655555555556</v>
+        <v>0.002195666666666664</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1520084062003005</v>
+        <v>0.04685794134046719</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>300</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>0.08891113640103362</v>
+        <v>0.02908624540066244</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>-0.4240208095423284</v>
+        <v>5.722071434572147</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>0.6632818910631735</v>
+        <v>35.01731264748563</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>0.8396769453491302</v>
+        <v>0.2613037285559408</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -1069,7 +869,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.68466667</v>
+        <v>1.586</v>
       </c>
     </row>
     <row r="11">
@@ -1079,7 +879,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.68640614</v>
+        <v>1.59964919</v>
       </c>
     </row>
     <row r="12">
@@ -1089,7 +889,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.023183835</v>
+        <v>0.00220301003</v>
       </c>
     </row>
     <row r="13">
@@ -1099,7 +899,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0230982802</v>
+        <v>0.00193312182</v>
       </c>
     </row>
     <row r="14">
@@ -1109,7 +909,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.152262389</v>
+        <v>0.0469362337</v>
       </c>
     </row>
     <row r="15">
@@ -1119,7 +919,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.151981184</v>
+        <v>0.0439672813</v>
       </c>
     </row>
     <row r="16">
@@ -1129,7 +929,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.709666666666667</v>
+        <v>1.611</v>
       </c>
     </row>
     <row r="17">
@@ -1139,7 +939,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.02310655555555556</v>
+        <v>0.002195666666666664</v>
       </c>
     </row>
     <row r="18">
@@ -1149,7 +949,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1520084062003005</v>
+        <v>0.04685794134046719</v>
       </c>
     </row>
     <row r="19">
@@ -1159,7 +959,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="20">
@@ -1169,7 +969,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="21">
@@ -1189,7 +989,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.08891113640103362</v>
+        <v>0.02908624540066244</v>
       </c>
     </row>
     <row r="23">
@@ -1199,7 +999,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.4240208095423284</v>
+        <v>5.722071434572147</v>
       </c>
     </row>
     <row r="24">
@@ -1209,7 +1009,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6632818910631735</v>
+        <v>35.01731264748563</v>
       </c>
     </row>
     <row r="25">
@@ -1219,7 +1019,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.8396769453491302</v>
+        <v>0.2613037285559408</v>
       </c>
     </row>
     <row r="26">

</xml_diff>